<commit_message>
new files for battle, empty js functions (or non-existent)
</commit_message>
<xml_diff>
--- a/resources/gameInfo/positionIdMap.xlsx
+++ b/resources/gameInfo/positionIdMap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>55-64</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>bought' troops zone is 118</t>
+  </si>
+  <si>
+    <t>Battle Zone Popup</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>buttons</t>
   </si>
 </sst>
 </file>
@@ -337,6 +346,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>613138</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11506200" y="1885950"/>
+          <a:ext cx="1943100" cy="2499088"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -628,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CJ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,6 +759,9 @@
       </c>
       <c r="L2" s="10"/>
       <c r="M2" s="11"/>
+      <c r="W2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:88" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
@@ -769,6 +824,9 @@
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="11"/>
+      <c r="AL4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:88" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -800,6 +858,12 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="11"/>
+      <c r="AK5">
+        <v>4</v>
+      </c>
+      <c r="AN5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:88" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -833,6 +897,12 @@
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="11"/>
+      <c r="AL6">
+        <v>6</v>
+      </c>
+      <c r="AM6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:88" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -866,6 +936,12 @@
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="11"/>
+      <c r="AK7">
+        <v>2</v>
+      </c>
+      <c r="AN7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:88" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
@@ -901,6 +977,9 @@
       <c r="M8" s="13"/>
       <c r="O8" s="8" t="s">
         <v>14</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:88" x14ac:dyDescent="0.3">
@@ -6239,5 +6318,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated popup and news stuff
</commit_message>
<xml_diff>
--- a/resources/gameInfo/positionIdMap.xlsx
+++ b/resources/gameInfo/positionIdMap.xlsx
@@ -305,6 +305,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -325,16 +331,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -683,14 +683,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CJ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="13" width="10.77734375" customWidth="1"/>
+    <col min="2" max="12" width="10.77734375" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" customWidth="1"/>
     <col min="14" max="14" width="4.33203125" customWidth="1"/>
     <col min="15" max="15" width="4.77734375" customWidth="1"/>
     <col min="16" max="16" width="4.33203125" customWidth="1"/>
@@ -698,11 +699,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:88" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="3">
         <v>0</v>
       </c>
@@ -733,10 +734,10 @@
       <c r="M1" s="6"/>
     </row>
     <row r="2" spans="1:88" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="16" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="4">
@@ -745,31 +746,31 @@
       <c r="F2" s="4">
         <v>10</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="4">
         <v>11</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="4">
         <v>12</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="10"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
       <c r="W2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:88" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="4">
         <v>13</v>
       </c>
@@ -779,7 +780,7 @@
       <c r="F3" s="4">
         <v>15</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="4">
@@ -791,9 +792,9 @@
       <c r="J3" s="4">
         <v>18</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:88" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
@@ -806,7 +807,7 @@
       <c r="D4" s="4">
         <v>21</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="4">
@@ -818,15 +819,15 @@
       <c r="H4" s="4">
         <v>24</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="9" t="s">
         <v>15</v>
       </c>
       <c r="J4" s="4">
         <v>25</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="12"/>
       <c r="AL4" t="s">
         <v>2</v>
       </c>
@@ -836,17 +837,17 @@
       <c r="B5" s="4">
         <v>26</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="4">
         <v>27</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="4">
         <v>28</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="4">
@@ -858,9 +859,9 @@
       <c r="J5" s="4">
         <v>31</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="10"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="12"/>
       <c r="AK5">
         <v>4</v>
       </c>
@@ -882,24 +883,24 @@
       <c r="E6" s="4">
         <v>35</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="10">
         <v>36</v>
       </c>
       <c r="H6" s="4">
         <v>37</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="9" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="4">
         <v>38</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="10"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="12"/>
       <c r="AL6">
         <v>6</v>
       </c>
@@ -915,7 +916,7 @@
       <c r="C7" s="4">
         <v>40</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="4">
@@ -924,7 +925,7 @@
       <c r="F7" s="4">
         <v>42</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="4">
@@ -936,9 +937,9 @@
       <c r="J7" s="4">
         <v>45</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="10"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="12"/>
       <c r="AK7">
         <v>2</v>
       </c>
@@ -975,9 +976,9 @@
       <c r="J8" s="5">
         <v>54</v>
       </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="12"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14"/>
       <c r="O8" s="7" t="s">
         <v>0</v>
       </c>

</xml_diff>